<commit_message>
Ajout EDT S6 25-26.
</commit_message>
<xml_diff>
--- a/BC.xlsx
+++ b/BC.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t xml:space="preserve">Semaine : </t>
   </si>
@@ -32,22 +32,34 @@
     <t>13:30</t>
   </si>
   <si>
+    <t>U3-Amphi</t>
+  </si>
+  <si>
     <t>TYPE_COURS</t>
   </si>
   <si>
     <t>jeudi</t>
   </si>
   <si>
+    <t>U3-110</t>
+  </si>
+  <si>
     <t>15:45</t>
   </si>
   <si>
     <t>mardi</t>
   </si>
   <si>
+    <t>U3-109</t>
+  </si>
+  <si>
     <t>vendredi</t>
   </si>
   <si>
     <t>10:0</t>
+  </si>
+  <si>
+    <t>U3-4</t>
   </si>
   <si>
     <t>ESE (KRTX9AC1)</t>
@@ -138,10 +150,12 @@
       <c r="E3" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F3" s="0"/>
+      <c r="F3" t="s" s="0">
+        <v>6</v>
+      </c>
       <c r="G3" s="0"/>
       <c r="H3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="0"/>
     </row>
@@ -158,7 +172,7 @@
         <v>45932.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -177,10 +191,12 @@
       <c r="E6" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F6" s="0"/>
+      <c r="F6" t="s" s="0">
+        <v>9</v>
+      </c>
       <c r="G6" s="0"/>
       <c r="H6" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6" s="0"/>
     </row>
@@ -195,15 +211,17 @@
         <v>4</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F7" s="0"/>
+      <c r="F7" t="s" s="0">
+        <v>9</v>
+      </c>
       <c r="G7" s="0"/>
       <c r="H7" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I7" s="0"/>
     </row>
@@ -220,7 +238,7 @@
         <v>45937.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -239,10 +257,12 @@
       <c r="E10" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F10" s="0"/>
+      <c r="F10" t="s" s="0">
+        <v>9</v>
+      </c>
       <c r="G10" s="0"/>
       <c r="H10" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I10" s="0"/>
     </row>
@@ -259,7 +279,7 @@
         <v>45944.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -278,10 +298,12 @@
       <c r="E13" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F13" s="0"/>
+      <c r="F13" t="s" s="0">
+        <v>12</v>
+      </c>
       <c r="G13" s="0"/>
       <c r="H13" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I13" s="0"/>
     </row>
@@ -298,7 +320,7 @@
         <v>45954.0</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -312,21 +334,23 @@
         <v>4</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E16" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F16" s="0"/>
+      <c r="F16" t="s" s="0">
+        <v>15</v>
+      </c>
       <c r="G16" s="0"/>
       <c r="H16" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I16" s="0"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>3</v>
@@ -340,10 +364,12 @@
       <c r="E17" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="F17" s="0"/>
+      <c r="F17" t="s" s="0">
+        <v>6</v>
+      </c>
       <c r="G17" s="0"/>
       <c r="H17" t="s" s="0">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I17" s="0"/>
     </row>

</xml_diff>